<commit_message>
Aanpassing dossier en timesheet
</commit_message>
<xml_diff>
--- a/docs/timesheet_ellen_tijtgat.xlsx
+++ b/docs/timesheet_ellen_tijtgat.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Datum</t>
   </si>
@@ -89,7 +89,13 @@
     <t>1u</t>
   </si>
   <si>
-    <t>Totaal: 23u</t>
+    <t>Start omzetten html5 template naar drupal template</t>
+  </si>
+  <si>
+    <t>Afwerking drupal template + dossier aanpassen</t>
+  </si>
+  <si>
+    <t>Totaal: 28u</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,7 +479,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -586,6 +592,34 @@
       </c>
       <c r="D10" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>42692</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>42694</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NEW BACKUP 29/12 16u
</commit_message>
<xml_diff>
--- a/docs/timesheet_ellen_tijtgat.xlsx
+++ b/docs/timesheet_ellen_tijtgat.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Datum</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Tijd (u)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User navigatie enkel op de userpagina's laten zien </t>
+  </si>
+  <si>
+    <t>Slideshow op iedere aanbod/vraagpagina</t>
   </si>
 </sst>
 </file>
@@ -457,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,8 +522,8 @@
         <v>2</v>
       </c>
       <c r="F3" s="4">
-        <f>SUM(D2:D19)</f>
-        <v>51</v>
+        <f>SUM(D2:D21)</f>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -742,6 +748,34 @@
       </c>
       <c r="D19">
         <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>42732</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>42733</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New backup 03/01 10u
</commit_message>
<xml_diff>
--- a/docs/timesheet_ellen_tijtgat.xlsx
+++ b/docs/timesheet_ellen_tijtgat.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Datum</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Slideshow op iedere aanbod/vraagpagina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mijn aanbodpagina aangepast, footermenu, userlogin </t>
+  </si>
+  <si>
+    <t>Homepage, messages, accountpagina, algmene contacpagina, test online deployment (5u!!!!)</t>
   </si>
 </sst>
 </file>
@@ -463,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,8 +528,8 @@
         <v>2</v>
       </c>
       <c r="F3" s="4">
-        <f>SUM(D2:D21)</f>
-        <v>56</v>
+        <f>SUM(D2:D23)</f>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -776,6 +782,34 @@
       </c>
       <c r="D21">
         <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>42705</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>42706</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>